<commit_message>
remove registration, remove PDF library, permissions, XLS - warehouse name
</commit_message>
<xml_diff>
--- a/assets/files/export.xlsx
+++ b/assets/files/export.xlsx
@@ -15,27 +15,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>Product name</t>
-  </si>
-  <si>
-    <t>Product quantity</t>
-  </si>
-  <si>
-    <t>Unit price</t>
-  </si>
-  <si>
-    <t>Unit weight</t>
-  </si>
-  <si>
-    <t>About</t>
-  </si>
-  <si>
-    <t>Photo link</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+  <si>
+    <t>Sklad:</t>
+  </si>
+  <si>
+    <t>prvy</t>
+  </si>
+  <si>
+    <t>ID produktu</t>
+  </si>
+  <si>
+    <t>Meno produktu</t>
+  </si>
+  <si>
+    <t>Pocet</t>
+  </si>
+  <si>
+    <t>Cena za jednotku</t>
+  </si>
+  <si>
+    <t>Jednotková váha</t>
+  </si>
+  <si>
+    <t>Vlastnosti</t>
+  </si>
+  <si>
+    <t>Link na obrázok</t>
   </si>
   <si>
     <t>KAWA ER6N</t>
@@ -392,7 +398,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -404,69 +410,79 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D5">
         <v>8000</v>
       </c>
-      <c r="E2">
+      <c r="E5">
         <v>206</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D6">
         <v>90</v>
       </c>
-      <c r="E3">
+      <c r="E6">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>